<commit_message>
TVP-13   Analyze and create the highlevel microservices diagram
- Update high level design for Server side
</commit_message>
<xml_diff>
--- a/truyenvui-diagram.xlsx
+++ b/truyenvui-diagram.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>Business requirement</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>- Assigns each external request</t>
+  </si>
+  <si>
+    <t>III. Basic design - Will update during implementation</t>
   </si>
 </sst>
 </file>
@@ -330,52 +333,52 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -393,21 +396,64 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1249544</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>883</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="885825" y="11772900"/>
+          <a:ext cx="12679544" cy="6325483"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:K7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:K7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A3:K7"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Column1" dataDxfId="12"/>
-    <tableColumn id="2" name="Customer" dataDxfId="11"/>
-    <tableColumn id="3" name="Payment" dataDxfId="10"/>
-    <tableColumn id="4" name="Comics" dataDxfId="9"/>
-    <tableColumn id="5" name="Community" dataDxfId="8"/>
-    <tableColumn id="6" name="Blog" dataDxfId="7"/>
-    <tableColumn id="7" name="DataCollection" dataDxfId="6"/>
-    <tableColumn id="8" name="Notification" dataDxfId="5"/>
-    <tableColumn id="9" name="Employee - translator" dataDxfId="4"/>
-    <tableColumn id="10" name="Account" dataDxfId="3"/>
-    <tableColumn id="11" name="Promotion tool" dataDxfId="2"/>
+    <tableColumn id="1" name="Column1" dataDxfId="10"/>
+    <tableColumn id="2" name="Customer" dataDxfId="9"/>
+    <tableColumn id="3" name="Payment" dataDxfId="8"/>
+    <tableColumn id="4" name="Comics" dataDxfId="7"/>
+    <tableColumn id="5" name="Community" dataDxfId="6"/>
+    <tableColumn id="6" name="Blog" dataDxfId="5"/>
+    <tableColumn id="7" name="DataCollection" dataDxfId="4"/>
+    <tableColumn id="8" name="Notification" dataDxfId="3"/>
+    <tableColumn id="9" name="Employee - translator" dataDxfId="2"/>
+    <tableColumn id="10" name="Account" dataDxfId="1"/>
+    <tableColumn id="11" name="Promotion tool" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -678,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,8 +1050,10 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1071,8 +1119,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>